<commit_message>
update data input file
</commit_message>
<xml_diff>
--- a/hetrogeneous_salvo_model/hetrogeneous_salvo_data_input_tool.xlsx
+++ b/hetrogeneous_salvo_model/hetrogeneous_salvo_data_input_tool.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/crg/Documents/python/combat-salvo/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/crg/Documents/python/combat-salvo/hetrogeneous_salvo_model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0060AFBE-95D3-9E46-896C-C01744B60DA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B2A24670-C42F-9B40-BFAA-6EA1E2FC0D95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-44260" yWindow="1100" windowWidth="22760" windowHeight="21500" xr2:uid="{28BD746A-A938-6448-AA59-235D6646DB62}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20640" activeTab="1" xr2:uid="{28BD746A-A938-6448-AA59-235D6646DB62}"/>
   </bookViews>
   <sheets>
     <sheet name="blue" sheetId="1" r:id="rId1"/>
-    <sheet name="red" sheetId="3" r:id="rId2"/>
+    <sheet name="red" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="26">
   <si>
     <t>Formations</t>
   </si>
@@ -96,9 +96,6 @@
     <t>MRC Company</t>
   </si>
   <si>
-    <t>MB1256788930</t>
-  </si>
-  <si>
     <t>NA</t>
   </si>
   <si>
@@ -114,16 +111,10 @@
     <t>MB1256788970</t>
   </si>
   <si>
-    <t>MB1256788730</t>
+    <t>range</t>
   </si>
   <si>
-    <t>MB1256788430</t>
-  </si>
-  <si>
-    <t>ADA Company</t>
-  </si>
-  <si>
-    <t>Sensor Company</t>
+    <t>formation</t>
   </si>
 </sst>
 </file>
@@ -162,7 +153,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -186,7 +177,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
@@ -204,7 +195,7 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="medium">
@@ -222,9 +213,65 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -237,10 +284,10 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -249,10 +296,38 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -267,42 +342,8 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -312,36 +353,10 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -351,91 +366,7 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -445,7 +376,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -457,58 +388,40 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -532,14 +445,14 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>50799</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>596900</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>46181</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -554,8 +467,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6959600" y="2286000"/>
-          <a:ext cx="8432800" cy="4635500"/>
+          <a:off x="6988464" y="2763981"/>
+          <a:ext cx="8490527" cy="4798291"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1177,13 +1090,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>685800</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1257,23 +1170,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>482600</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:rowOff>50799</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>660400</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>596900</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:rowOff>46181</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="2" name="TextBox 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1C36242D-4A7D-074D-A8E6-6A48BB792684}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E742B2B-C5E4-0146-880F-2AD931A1B6DF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1281,8 +1194,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13627100" y="2819400"/>
-          <a:ext cx="8432800" cy="4635500"/>
+          <a:off x="6959600" y="2705099"/>
+          <a:ext cx="8432800" cy="4694382"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1894,6 +1807,80 @@
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
             <a:t>distraction factor for force [0,1].</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DEF7B074-EEEA-9F46-B53E-C4DF08F6736E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7226300" y="482600"/>
+          <a:ext cx="3073400" cy="774700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>-Need VBA</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> code to automate the units in columns D:F </a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -2203,10 +2190,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D16411E9-895C-514F-9F09-12EF137F6C1B}">
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2216,684 +2203,792 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="D1" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="F1" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="30" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="21"/>
+      <c r="B3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="21"/>
+      <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
+      <c r="D4" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="21"/>
+      <c r="B5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="2">
+        <v>8000</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="21"/>
+      <c r="B6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="2">
+        <v>4</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="21"/>
+      <c r="B7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="2">
+        <v>8</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="21"/>
+      <c r="B8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="9">
+        <v>2</v>
+      </c>
+      <c r="E8" s="9">
+        <v>2</v>
+      </c>
+      <c r="F8" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="21"/>
+      <c r="B9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="E9" s="9">
+        <v>0.25</v>
+      </c>
+      <c r="F9" s="12">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="21"/>
+      <c r="B10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="9">
+        <v>0</v>
+      </c>
+      <c r="E10" s="9">
+        <v>0</v>
+      </c>
+      <c r="F10" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="21"/>
+      <c r="B11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="9">
+        <v>2</v>
+      </c>
+      <c r="E11" s="9">
+        <v>2</v>
+      </c>
+      <c r="F11" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="21"/>
+      <c r="B12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="9">
+        <v>0</v>
+      </c>
+      <c r="E12" s="9">
+        <v>0</v>
+      </c>
+      <c r="F12" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="21"/>
+      <c r="B13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="9">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="E13" s="9">
+        <v>1</v>
+      </c>
+      <c r="F13" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="21"/>
+      <c r="B14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="9">
+        <v>1</v>
+      </c>
+      <c r="E14" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="F14" s="12">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="22"/>
+      <c r="B15" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="14">
+        <v>0.7</v>
+      </c>
+      <c r="E15" s="14">
+        <v>1</v>
+      </c>
+      <c r="F15" s="15">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="F16" s="17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="21"/>
+      <c r="B17" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C17" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" s="25" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="4"/>
-      <c r="B3" s="1" t="s">
+      <c r="D17" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F17" s="18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="21"/>
+      <c r="B18" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C18" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="21"/>
+      <c r="B19" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" s="16" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="4"/>
-      <c r="B4" s="1" t="s">
+      <c r="C19" s="2">
+        <v>8000</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="21"/>
+      <c r="B20" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C20" s="2">
         <v>4</v>
       </c>
-      <c r="D4" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="16" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="4"/>
-      <c r="B5" s="3" t="s">
+      <c r="D20" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="21"/>
+      <c r="B21" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C21" s="2">
         <v>8</v>
       </c>
-      <c r="D5" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" s="16" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="4"/>
-      <c r="B6" s="1" t="s">
+      <c r="D21" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F21" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="21"/>
+      <c r="B22" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="13">
+      <c r="C22" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D22" s="9">
         <v>2</v>
       </c>
-      <c r="E6" s="13">
+      <c r="E22" s="9">
         <v>2</v>
       </c>
-      <c r="F6" s="16">
+      <c r="F22" s="12">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="4"/>
-      <c r="B7" s="1" t="s">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="21"/>
+      <c r="B23" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="13">
+      <c r="C23" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23" s="9">
         <v>0.5</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E23" s="9">
         <v>0.25</v>
       </c>
-      <c r="F7" s="16">
+      <c r="F23" s="12">
         <v>0.25</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="4"/>
-      <c r="B8" s="3" t="s">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="21"/>
+      <c r="B24" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="13">
+      <c r="C24" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D24" s="9">
         <v>0</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E24" s="9">
         <v>0</v>
       </c>
-      <c r="F8" s="16">
+      <c r="F24" s="12">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="4"/>
-      <c r="B9" s="1" t="s">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="21"/>
+      <c r="B25" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" s="13">
+      <c r="C25" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D25" s="9">
         <v>2</v>
       </c>
-      <c r="E9" s="13">
+      <c r="E25" s="9">
         <v>2</v>
       </c>
-      <c r="F9" s="16">
+      <c r="F25" s="12">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="4"/>
-      <c r="B10" s="1" t="s">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="21"/>
+      <c r="B26" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="13">
+      <c r="C26" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D26" s="9">
         <v>0</v>
       </c>
-      <c r="E10" s="13">
+      <c r="E26" s="9">
         <v>0</v>
       </c>
-      <c r="F10" s="16">
+      <c r="F26" s="12">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="4"/>
-      <c r="B11" s="1" t="s">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="21"/>
+      <c r="B27" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" s="13">
+      <c r="C27" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D27" s="9">
         <v>1</v>
       </c>
-      <c r="E11" s="13">
+      <c r="E27" s="9">
         <v>1</v>
       </c>
-      <c r="F11" s="16">
+      <c r="F27" s="12">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="4"/>
-      <c r="B12" s="1" t="s">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="21"/>
+      <c r="B28" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" s="13">
+      <c r="C28" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D28" s="9">
         <v>1</v>
       </c>
-      <c r="E12" s="13">
+      <c r="E28" s="9">
         <v>0.8</v>
       </c>
-      <c r="F12" s="16">
+      <c r="F28" s="12">
         <v>0.7</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
-      <c r="B13" s="6" t="s">
+    <row r="29" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="22"/>
+      <c r="B29" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13" s="18">
+      <c r="C29" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D29" s="14">
         <v>0.7</v>
       </c>
-      <c r="E13" s="18">
+      <c r="E29" s="14">
         <v>1</v>
       </c>
-      <c r="F13" s="19">
+      <c r="F29" s="15">
         <v>0.8</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="20" t="s">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="B30" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C30" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E30" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F30" s="18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" s="21"/>
+      <c r="B31" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D31" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E31" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F31" s="18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" s="21"/>
+      <c r="B32" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F32" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" s="21"/>
+      <c r="B33" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C33" s="2">
+        <v>8000</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E33" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F33" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" s="21"/>
+      <c r="B34" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34" s="2">
+        <v>4</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E34" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F34" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" s="21"/>
+      <c r="B35" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C35" s="2">
+        <v>8</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E35" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F35" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" s="21"/>
+      <c r="B36" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D36" s="9">
         <v>2</v>
       </c>
-      <c r="B14" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="D14" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="E14" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="F14" s="24" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="4"/>
-      <c r="B15" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D15" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="E15" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="F15" s="16" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="4"/>
-      <c r="B16" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16" s="2">
+      <c r="E36" s="9">
+        <v>2</v>
+      </c>
+      <c r="F36" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" s="21"/>
+      <c r="B37" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D37" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="E37" s="9">
+        <v>0.25</v>
+      </c>
+      <c r="F37" s="12">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" s="21"/>
+      <c r="B38" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D38" s="9">
+        <v>0</v>
+      </c>
+      <c r="E38" s="9">
+        <v>0</v>
+      </c>
+      <c r="F38" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" s="21"/>
+      <c r="B39" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="E16" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="F16" s="16" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="4"/>
-      <c r="B17" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17" s="2">
-        <v>8</v>
-      </c>
-      <c r="D17" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="E17" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="F17" s="16" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="4"/>
-      <c r="B18" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D18" s="13">
+      <c r="C39" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D39" s="9">
+        <v>2</v>
+      </c>
+      <c r="E39" s="9">
+        <v>2</v>
+      </c>
+      <c r="F39" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" s="21"/>
+      <c r="B40" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D40" s="9">
         <v>0</v>
       </c>
-      <c r="E18" s="13">
+      <c r="E40" s="9">
         <v>0</v>
       </c>
-      <c r="F18" s="16">
+      <c r="F40" s="12">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="4"/>
-      <c r="B19" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D19" s="13">
-        <v>0</v>
-      </c>
-      <c r="E19" s="13">
-        <v>0</v>
-      </c>
-      <c r="F19" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="4"/>
-      <c r="B20" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D20" s="13">
-        <v>3</v>
-      </c>
-      <c r="E20" s="13">
-        <v>3</v>
-      </c>
-      <c r="F20" s="16">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="4"/>
-      <c r="B21" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D21" s="13">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" s="21"/>
+      <c r="B41" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D41" s="9">
         <v>1</v>
       </c>
-      <c r="E21" s="13">
+      <c r="E41" s="9">
         <v>1</v>
       </c>
-      <c r="F21" s="16">
+      <c r="F41" s="12">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="4"/>
-      <c r="B22" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D22" s="13">
-        <v>0</v>
-      </c>
-      <c r="E22" s="13">
-        <v>0</v>
-      </c>
-      <c r="F22" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="4"/>
-      <c r="B23" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D23" s="13">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" s="21"/>
+      <c r="B42" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D42" s="9">
         <v>1</v>
       </c>
-      <c r="E23" s="13">
+      <c r="E42" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="F42" s="12">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="22"/>
+      <c r="B43" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C43" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D43" s="14">
+        <v>0.7</v>
+      </c>
+      <c r="E43" s="14">
         <v>1</v>
       </c>
-      <c r="F23" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="4"/>
-      <c r="B24" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D24" s="13">
-        <v>1</v>
-      </c>
-      <c r="E24" s="13">
-        <v>1</v>
-      </c>
-      <c r="F24" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="5"/>
-      <c r="B25" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C25" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="D25" s="18">
-        <v>0.7</v>
-      </c>
-      <c r="E25" s="18">
-        <v>1</v>
-      </c>
-      <c r="F25" s="19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="B26" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="C26" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="D26" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="E26" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="F26" s="24" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="4"/>
-      <c r="B27" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D27" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="E27" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="F27" s="16" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" s="4"/>
-      <c r="B28" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C28" s="2">
-        <v>12</v>
-      </c>
-      <c r="D28" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="E28" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="F28" s="16" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" s="4"/>
-      <c r="B29" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C29" s="2">
-        <v>8</v>
-      </c>
-      <c r="D29" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="E29" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="F29" s="16" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30" s="4"/>
-      <c r="B30" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D30" s="13">
-        <v>0</v>
-      </c>
-      <c r="E30" s="13">
-        <v>0</v>
-      </c>
-      <c r="F30" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31" s="4"/>
-      <c r="B31" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D31" s="13">
-        <v>0</v>
-      </c>
-      <c r="E31" s="13">
-        <v>0</v>
-      </c>
-      <c r="F31" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" s="4"/>
-      <c r="B32" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D32" s="13">
-        <v>0</v>
-      </c>
-      <c r="E32" s="13">
-        <v>0</v>
-      </c>
-      <c r="F32" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33" s="4"/>
-      <c r="B33" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D33" s="13">
-        <v>1</v>
-      </c>
-      <c r="E33" s="13">
-        <v>1</v>
-      </c>
-      <c r="F33" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34" s="4"/>
-      <c r="B34" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D34" s="13">
-        <v>1</v>
-      </c>
-      <c r="E34" s="13">
-        <v>1</v>
-      </c>
-      <c r="F34" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35" s="4"/>
-      <c r="B35" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D35" s="13">
-        <v>1</v>
-      </c>
-      <c r="E35" s="13">
-        <v>1</v>
-      </c>
-      <c r="F35" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36" s="4"/>
-      <c r="B36" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D36" s="13">
-        <v>1</v>
-      </c>
-      <c r="E36" s="13">
-        <v>1</v>
-      </c>
-      <c r="F36" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="5"/>
-      <c r="B37" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C37" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="D37" s="18">
-        <v>0.7</v>
-      </c>
-      <c r="E37" s="18">
-        <v>1</v>
-      </c>
-      <c r="F37" s="19">
-        <v>1</v>
+      <c r="F43" s="15">
+        <v>0.8</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A2:A13"/>
-    <mergeCell ref="A14:A25"/>
-    <mergeCell ref="A26:A37"/>
+    <mergeCell ref="A2:A15"/>
+    <mergeCell ref="A16:A29"/>
+    <mergeCell ref="A30:A43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2901,11 +2996,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE3A889B-78C4-6146-9A66-A6BD2CB3C889}">
-  <dimension ref="A1:F37"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34DC9FCA-E070-744D-A42B-CA7E9735447B}">
+  <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2915,684 +3010,792 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="D1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="E1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="30" t="s">
+      <c r="F1" s="8" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="21"/>
+      <c r="B3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="21"/>
+      <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="21"/>
+      <c r="B5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="2">
+        <v>8000</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="21"/>
+      <c r="B6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="2">
+        <v>4</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="21"/>
+      <c r="B7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="2">
+        <v>8</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="21"/>
+      <c r="B8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="9">
+        <v>2</v>
+      </c>
+      <c r="E8" s="9">
+        <v>2</v>
+      </c>
+      <c r="F8" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="21"/>
+      <c r="B9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="E9" s="9">
+        <v>0.25</v>
+      </c>
+      <c r="F9" s="12">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="21"/>
+      <c r="B10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="9">
+        <v>0</v>
+      </c>
+      <c r="E10" s="9">
+        <v>0</v>
+      </c>
+      <c r="F10" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="21"/>
+      <c r="B11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="9">
+        <v>2</v>
+      </c>
+      <c r="E11" s="9">
+        <v>2</v>
+      </c>
+      <c r="F11" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="21"/>
+      <c r="B12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="9">
+        <v>0</v>
+      </c>
+      <c r="E12" s="9">
+        <v>0</v>
+      </c>
+      <c r="F12" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="21"/>
+      <c r="B13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="9">
+        <v>1</v>
+      </c>
+      <c r="E13" s="9">
+        <v>1</v>
+      </c>
+      <c r="F13" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="21"/>
+      <c r="B14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="9">
+        <v>1</v>
+      </c>
+      <c r="E14" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="F14" s="12">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="22"/>
+      <c r="B15" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="14">
+        <v>0.7</v>
+      </c>
+      <c r="E15" s="14">
+        <v>1</v>
+      </c>
+      <c r="F15" s="15">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B16" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="F16" s="17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="21"/>
+      <c r="B17" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C17" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" s="24" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="4"/>
-      <c r="B3" s="1" t="s">
+      <c r="D17" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F17" s="18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="21"/>
+      <c r="B18" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" s="16" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="4"/>
-      <c r="B4" s="1" t="s">
+      <c r="C18" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="21"/>
+      <c r="B19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="2">
+        <v>8000</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="21"/>
+      <c r="B20" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="12">
+      <c r="C20" s="2">
+        <v>4</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="21"/>
+      <c r="B21" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="2">
+        <v>8</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F21" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="21"/>
+      <c r="B22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D22" s="9">
+        <v>2</v>
+      </c>
+      <c r="E22" s="9">
+        <v>2</v>
+      </c>
+      <c r="F22" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="21"/>
+      <c r="B23" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="E23" s="9">
+        <v>0.25</v>
+      </c>
+      <c r="F23" s="12">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="21"/>
+      <c r="B24" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D24" s="9">
+        <v>0</v>
+      </c>
+      <c r="E24" s="9">
+        <v>0</v>
+      </c>
+      <c r="F24" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="21"/>
+      <c r="B25" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="16" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="4"/>
-      <c r="B5" s="3" t="s">
+      <c r="C25" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D25" s="9">
+        <v>2</v>
+      </c>
+      <c r="E25" s="9">
+        <v>2</v>
+      </c>
+      <c r="F25" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="21"/>
+      <c r="B26" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D26" s="9">
+        <v>0</v>
+      </c>
+      <c r="E26" s="9">
+        <v>0</v>
+      </c>
+      <c r="F26" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="21"/>
+      <c r="B27" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D27" s="9">
+        <v>1</v>
+      </c>
+      <c r="E27" s="9">
+        <v>1</v>
+      </c>
+      <c r="F27" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="21"/>
+      <c r="B28" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D28" s="9">
+        <v>1</v>
+      </c>
+      <c r="E28" s="9">
+        <v>0.8</v>
+      </c>
+      <c r="F28" s="12">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="22"/>
+      <c r="B29" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D29" s="14">
+        <v>0.7</v>
+      </c>
+      <c r="E29" s="14">
+        <v>1</v>
+      </c>
+      <c r="F29" s="15">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B30" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C30" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E30" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F30" s="18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" s="21"/>
+      <c r="B31" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D31" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E31" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F31" s="18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" s="21"/>
+      <c r="B32" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F32" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" s="21"/>
+      <c r="B33" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C33" s="2">
+        <v>8000</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E33" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F33" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" s="21"/>
+      <c r="B34" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34" s="2">
+        <v>4</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E34" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F34" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" s="21"/>
+      <c r="B35" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="12">
+      <c r="C35" s="2">
         <v>8</v>
       </c>
-      <c r="D5" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" s="16" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="4"/>
-      <c r="B6" s="1" t="s">
+      <c r="D35" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E35" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F35" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" s="21"/>
+      <c r="B36" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="13">
+      <c r="C36" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D36" s="9">
         <v>2</v>
       </c>
-      <c r="E6" s="13">
+      <c r="E36" s="9">
         <v>2</v>
       </c>
-      <c r="F6" s="16">
+      <c r="F36" s="12">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="4"/>
-      <c r="B7" s="1" t="s">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" s="21"/>
+      <c r="B37" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="13">
+      <c r="C37" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D37" s="9">
         <v>0.5</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E37" s="9">
         <v>0.25</v>
       </c>
-      <c r="F7" s="16">
+      <c r="F37" s="12">
         <v>0.25</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="4"/>
-      <c r="B8" s="3" t="s">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" s="21"/>
+      <c r="B38" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="13">
+      <c r="C38" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D38" s="9">
         <v>0</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E38" s="9">
         <v>0</v>
       </c>
-      <c r="F8" s="16">
+      <c r="F38" s="12">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="4"/>
-      <c r="B9" s="1" t="s">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" s="21"/>
+      <c r="B39" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" s="13">
+      <c r="C39" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D39" s="9">
         <v>2</v>
       </c>
-      <c r="E9" s="13">
+      <c r="E39" s="9">
         <v>2</v>
       </c>
-      <c r="F9" s="16">
+      <c r="F39" s="12">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="4"/>
-      <c r="B10" s="1" t="s">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" s="21"/>
+      <c r="B40" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="13">
+      <c r="C40" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D40" s="9">
         <v>0</v>
       </c>
-      <c r="E10" s="13">
+      <c r="E40" s="9">
         <v>0</v>
       </c>
-      <c r="F10" s="16">
+      <c r="F40" s="12">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="4"/>
-      <c r="B11" s="1" t="s">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" s="21"/>
+      <c r="B41" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" s="13">
+      <c r="C41" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D41" s="9">
         <v>1</v>
       </c>
-      <c r="E11" s="13">
+      <c r="E41" s="9">
         <v>1</v>
       </c>
-      <c r="F11" s="16">
+      <c r="F41" s="12">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="4"/>
-      <c r="B12" s="1" t="s">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" s="21"/>
+      <c r="B42" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" s="13">
+      <c r="C42" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D42" s="9">
         <v>1</v>
       </c>
-      <c r="E12" s="13">
+      <c r="E42" s="9">
         <v>0.8</v>
       </c>
-      <c r="F12" s="16">
+      <c r="F42" s="12">
         <v>0.7</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
-      <c r="B13" s="6" t="s">
+    <row r="43" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="22"/>
+      <c r="B43" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13" s="18">
+      <c r="C43" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D43" s="14">
         <v>0.7</v>
       </c>
-      <c r="E13" s="18">
+      <c r="E43" s="14">
         <v>1</v>
       </c>
-      <c r="F13" s="19">
+      <c r="F43" s="15">
         <v>0.8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="B14" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="E14" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="F14" s="24" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="4"/>
-      <c r="B15" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="D15" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="E15" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="F15" s="16" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="4"/>
-      <c r="B16" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16" s="12">
-        <v>12</v>
-      </c>
-      <c r="D16" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="E16" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="F16" s="16" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="4"/>
-      <c r="B17" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17" s="12">
-        <v>8</v>
-      </c>
-      <c r="D17" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="E17" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="F17" s="16" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="4"/>
-      <c r="B18" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C18" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D18" s="13">
-        <v>0</v>
-      </c>
-      <c r="E18" s="13">
-        <v>0</v>
-      </c>
-      <c r="F18" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="4"/>
-      <c r="B19" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C19" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D19" s="13">
-        <v>0</v>
-      </c>
-      <c r="E19" s="13">
-        <v>0</v>
-      </c>
-      <c r="F19" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="4"/>
-      <c r="B20" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C20" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D20" s="13">
-        <v>3</v>
-      </c>
-      <c r="E20" s="13">
-        <v>3</v>
-      </c>
-      <c r="F20" s="16">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="4"/>
-      <c r="B21" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C21" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D21" s="13">
-        <v>1</v>
-      </c>
-      <c r="E21" s="13">
-        <v>1</v>
-      </c>
-      <c r="F21" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="4"/>
-      <c r="B22" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C22" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D22" s="13">
-        <v>0</v>
-      </c>
-      <c r="E22" s="13">
-        <v>0</v>
-      </c>
-      <c r="F22" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="4"/>
-      <c r="B23" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C23" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D23" s="13">
-        <v>1</v>
-      </c>
-      <c r="E23" s="13">
-        <v>1</v>
-      </c>
-      <c r="F23" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="4"/>
-      <c r="B24" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C24" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D24" s="13">
-        <v>1</v>
-      </c>
-      <c r="E24" s="13">
-        <v>1</v>
-      </c>
-      <c r="F24" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="5"/>
-      <c r="B25" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C25" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="D25" s="18">
-        <v>0.7</v>
-      </c>
-      <c r="E25" s="18">
-        <v>1</v>
-      </c>
-      <c r="F25" s="19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="B26" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="C26" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="D26" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="E26" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="F26" s="24" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="4"/>
-      <c r="B27" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C27" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="D27" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="E27" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="F27" s="16" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" s="4"/>
-      <c r="B28" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C28" s="12">
-        <v>12</v>
-      </c>
-      <c r="D28" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="E28" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="F28" s="16" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" s="4"/>
-      <c r="B29" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C29" s="12">
-        <v>8</v>
-      </c>
-      <c r="D29" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="E29" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="F29" s="16" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30" s="4"/>
-      <c r="B30" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C30" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D30" s="13">
-        <v>0</v>
-      </c>
-      <c r="E30" s="13">
-        <v>0</v>
-      </c>
-      <c r="F30" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31" s="4"/>
-      <c r="B31" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C31" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D31" s="13">
-        <v>0</v>
-      </c>
-      <c r="E31" s="13">
-        <v>0</v>
-      </c>
-      <c r="F31" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" s="4"/>
-      <c r="B32" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C32" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D32" s="13">
-        <v>0</v>
-      </c>
-      <c r="E32" s="13">
-        <v>0</v>
-      </c>
-      <c r="F32" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33" s="4"/>
-      <c r="B33" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C33" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D33" s="13">
-        <v>1</v>
-      </c>
-      <c r="E33" s="13">
-        <v>1</v>
-      </c>
-      <c r="F33" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34" s="4"/>
-      <c r="B34" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C34" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D34" s="13">
-        <v>1</v>
-      </c>
-      <c r="E34" s="13">
-        <v>1</v>
-      </c>
-      <c r="F34" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35" s="4"/>
-      <c r="B35" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C35" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D35" s="13">
-        <v>1</v>
-      </c>
-      <c r="E35" s="13">
-        <v>1</v>
-      </c>
-      <c r="F35" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36" s="4"/>
-      <c r="B36" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C36" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D36" s="13">
-        <v>1</v>
-      </c>
-      <c r="E36" s="13">
-        <v>1</v>
-      </c>
-      <c r="F36" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="5"/>
-      <c r="B37" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C37" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="D37" s="18">
-        <v>0.7</v>
-      </c>
-      <c r="E37" s="18">
-        <v>1</v>
-      </c>
-      <c r="F37" s="19">
-        <v>1</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A2:A13"/>
-    <mergeCell ref="A14:A25"/>
-    <mergeCell ref="A26:A37"/>
+    <mergeCell ref="A2:A15"/>
+    <mergeCell ref="A16:A29"/>
+    <mergeCell ref="A30:A43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
build off and def matrix
</commit_message>
<xml_diff>
--- a/hetrogeneous_salvo_model/hetrogeneous_salvo_data_input_tool.xlsx
+++ b/hetrogeneous_salvo_model/hetrogeneous_salvo_data_input_tool.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/crg/Documents/python/combat-salvo/hetrogeneous_salvo_model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC0EEB55-162A-274A-8F62-B6CF44F91254}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85608065-93DD-0248-8E3D-E8688E0EE9BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20640" xr2:uid="{28BD746A-A938-6448-AA59-235D6646DB62}"/>
+    <workbookView xWindow="-36460" yWindow="380" windowWidth="16920" windowHeight="20640" xr2:uid="{28BD746A-A938-6448-AA59-235D6646DB62}"/>
   </bookViews>
   <sheets>
     <sheet name="blue" sheetId="1" r:id="rId1"/>
@@ -2179,8 +2179,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D16411E9-895C-514F-9F09-12EF137F6C1B}">
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2418,13 +2418,13 @@
         <v>16</v>
       </c>
       <c r="D13" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F13" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -2654,13 +2654,13 @@
         <v>16</v>
       </c>
       <c r="D26" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E26" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F26" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -2690,13 +2690,13 @@
         <v>16</v>
       </c>
       <c r="D28" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E28" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F28" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -2962,13 +2962,13 @@
         <v>16</v>
       </c>
       <c r="D43" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E43" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F43" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
finished engagment class problem w defense matrix
</commit_message>
<xml_diff>
--- a/hetrogeneous_salvo_model/hetrogeneous_salvo_data_input_tool.xlsx
+++ b/hetrogeneous_salvo_model/hetrogeneous_salvo_data_input_tool.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/crg/Documents/python/combat-salvo/hetrogeneous_salvo_model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85608065-93DD-0248-8E3D-E8688E0EE9BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A00216A2-5FC2-D84E-B11D-B5A231AD1417}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-36460" yWindow="380" windowWidth="16920" windowHeight="20640" xr2:uid="{28BD746A-A938-6448-AA59-235D6646DB62}"/>
+    <workbookView xWindow="17260" yWindow="500" windowWidth="18580" windowHeight="20640" xr2:uid="{28BD746A-A938-6448-AA59-235D6646DB62}"/>
   </bookViews>
   <sheets>
     <sheet name="blue" sheetId="1" r:id="rId1"/>
     <sheet name="red" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -58,9 +58,6 @@
   </si>
   <si>
     <t>mgrs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">defense_capability </t>
   </si>
   <si>
     <t>fraction_engage</t>
@@ -119,6 +116,9 @@
   <si>
     <t>aimed_offense</t>
   </si>
+  <si>
+    <t>defense_capability</t>
+  </si>
 </sst>
 </file>
 
@@ -148,12 +148,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="15">
@@ -364,7 +370,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
@@ -372,41 +378,52 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2179,8 +2196,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D16411E9-895C-514F-9F09-12EF137F6C1B}">
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2197,171 +2214,171 @@
         <v>4</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>19</v>
-      </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="24" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="20"/>
+      <c r="A3" s="25"/>
       <c r="B3" s="9" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="20"/>
+      <c r="A4" s="25"/>
       <c r="B4" s="11" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="25"/>
+      <c r="B5" s="11" t="s">
         <v>20</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="20"/>
-      <c r="B5" s="11" t="s">
-        <v>21</v>
       </c>
       <c r="C5" s="12">
         <v>8000</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="20"/>
+      <c r="A6" s="25"/>
       <c r="B6" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C6" s="12">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="20"/>
+      <c r="A7" s="25"/>
       <c r="B7" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C7" s="12">
         <v>8</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F7" s="14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="20"/>
+      <c r="A8" s="25"/>
       <c r="B8" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C8" s="12">
         <v>8</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="20"/>
+      <c r="A9" s="25"/>
       <c r="B9" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D9" s="13">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="E9" s="13">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="F9" s="14">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="20"/>
+      <c r="A10" s="25"/>
       <c r="B10" s="11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D10" s="13">
         <v>0.5</v>
@@ -2374,30 +2391,30 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="20"/>
-      <c r="B11" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="13">
+      <c r="A11" s="25"/>
+      <c r="B11" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="22">
+        <v>0.3</v>
+      </c>
+      <c r="E11" s="22">
         <v>0</v>
       </c>
-      <c r="E11" s="13">
+      <c r="F11" s="23">
         <v>0</v>
       </c>
-      <c r="F11" s="14">
-        <v>0</v>
-      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="20"/>
+      <c r="A12" s="25"/>
       <c r="B12" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D12" s="13">
         <v>2</v>
@@ -2410,48 +2427,48 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="20"/>
+      <c r="A13" s="25"/>
       <c r="B13" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="13">
+        <v>1</v>
+      </c>
+      <c r="E13" s="13">
+        <v>1</v>
+      </c>
+      <c r="F13" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="25"/>
+      <c r="B14" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13" s="13">
-        <v>1</v>
-      </c>
-      <c r="E13" s="13">
-        <v>1</v>
-      </c>
-      <c r="F13" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="20"/>
-      <c r="B14" s="11" t="s">
+      <c r="C14" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="13">
+        <v>1</v>
+      </c>
+      <c r="E14" s="13">
+        <v>1</v>
+      </c>
+      <c r="F14" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="25"/>
+      <c r="B15" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="D14" s="13">
-        <v>1</v>
-      </c>
-      <c r="E14" s="13">
-        <v>1</v>
-      </c>
-      <c r="F14" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="20"/>
-      <c r="B15" s="11" t="s">
-        <v>12</v>
-      </c>
       <c r="C15" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D15" s="13">
         <v>1</v>
@@ -2464,12 +2481,12 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="21"/>
+      <c r="A16" s="26"/>
       <c r="B16" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D16" s="17">
         <v>0.7</v>
@@ -2482,158 +2499,158 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="19" t="s">
+      <c r="A17" s="24" t="s">
         <v>2</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>2</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="20"/>
+      <c r="A18" s="25"/>
       <c r="B18" s="9" t="s">
         <v>5</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="20"/>
+      <c r="A19" s="25"/>
       <c r="B19" s="11" t="s">
         <v>6</v>
       </c>
       <c r="C19" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F19" s="14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="25"/>
+      <c r="B20" s="11" t="s">
         <v>20</v>
-      </c>
-      <c r="D19" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E19" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="F19" s="14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="20"/>
-      <c r="B20" s="11" t="s">
-        <v>21</v>
       </c>
       <c r="C20" s="12">
         <v>8000</v>
       </c>
       <c r="D20" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E20" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F20" s="14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="20"/>
+      <c r="A21" s="25"/>
       <c r="B21" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C21" s="12">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="D21" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E21" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F21" s="14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="20"/>
+      <c r="A22" s="25"/>
       <c r="B22" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C22" s="12">
         <v>8</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E22" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F22" s="14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="20"/>
+      <c r="A23" s="25"/>
       <c r="B23" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C23" s="12">
         <v>8</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E23" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F23" s="14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="20"/>
+      <c r="A24" s="25"/>
       <c r="B24" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D24" s="13">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="E24" s="13">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="F24" s="14">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="20"/>
+      <c r="A25" s="25"/>
       <c r="B25" s="11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D25" s="13">
         <v>0.5</v>
@@ -2646,30 +2663,30 @@
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="20"/>
-      <c r="B26" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C26" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="D26" s="13">
-        <v>1</v>
-      </c>
-      <c r="E26" s="13">
-        <v>1</v>
-      </c>
-      <c r="F26" s="14">
-        <v>1</v>
+      <c r="A26" s="25"/>
+      <c r="B26" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="D26" s="22">
+        <v>0</v>
+      </c>
+      <c r="E26" s="22">
+        <v>0</v>
+      </c>
+      <c r="F26" s="23">
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="20"/>
+      <c r="A27" s="25"/>
       <c r="B27" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D27" s="13">
         <v>2</v>
@@ -2682,48 +2699,48 @@
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" s="20"/>
+      <c r="A28" s="25"/>
       <c r="B28" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D28" s="13">
+        <v>0.2</v>
+      </c>
+      <c r="E28" s="13">
+        <v>0.2</v>
+      </c>
+      <c r="F28" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" s="25"/>
+      <c r="B29" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C28" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="D28" s="13">
-        <v>1</v>
-      </c>
-      <c r="E28" s="13">
-        <v>1</v>
-      </c>
-      <c r="F28" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" s="20"/>
-      <c r="B29" s="11" t="s">
+      <c r="C29" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D29" s="13">
+        <v>1</v>
+      </c>
+      <c r="E29" s="13">
+        <v>1</v>
+      </c>
+      <c r="F29" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" s="25"/>
+      <c r="B30" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C29" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="D29" s="13">
-        <v>1</v>
-      </c>
-      <c r="E29" s="13">
-        <v>1</v>
-      </c>
-      <c r="F29" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30" s="20"/>
-      <c r="B30" s="11" t="s">
-        <v>12</v>
-      </c>
       <c r="C30" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D30" s="13">
         <v>1</v>
@@ -2736,12 +2753,12 @@
       </c>
     </row>
     <row r="31" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="21"/>
+      <c r="A31" s="26"/>
       <c r="B31" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C31" s="16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D31" s="17">
         <v>0.7</v>
@@ -2754,158 +2771,158 @@
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" s="19" t="s">
+      <c r="A32" s="24" t="s">
         <v>3</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C32" s="6" t="s">
         <v>3</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F32" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33" s="20"/>
+      <c r="A33" s="25"/>
       <c r="B33" s="9" t="s">
         <v>5</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F33" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34" s="20"/>
+      <c r="A34" s="25"/>
       <c r="B34" s="11" t="s">
         <v>6</v>
       </c>
       <c r="C34" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D34" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E34" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F34" s="14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" s="25"/>
+      <c r="B35" s="11" t="s">
         <v>20</v>
-      </c>
-      <c r="D34" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E34" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="F34" s="14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35" s="20"/>
-      <c r="B35" s="11" t="s">
-        <v>21</v>
       </c>
       <c r="C35" s="12">
         <v>8000</v>
       </c>
       <c r="D35" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E35" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F35" s="14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36" s="20"/>
+      <c r="A36" s="25"/>
       <c r="B36" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C36" s="12">
-        <v>4</v>
+        <v>22</v>
+      </c>
+      <c r="C36" s="19">
+        <v>15</v>
       </c>
       <c r="D36" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E36" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F36" s="14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37" s="20"/>
+      <c r="A37" s="25"/>
       <c r="B37" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C37" s="12">
         <v>8</v>
       </c>
       <c r="D37" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E37" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F37" s="14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38" s="20"/>
+      <c r="A38" s="25"/>
       <c r="B38" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C38" s="12">
         <v>8</v>
       </c>
       <c r="D38" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E38" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F38" s="14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A39" s="20"/>
+      <c r="A39" s="25"/>
       <c r="B39" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D39" s="13">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="E39" s="13">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="F39" s="14">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A40" s="20"/>
+      <c r="A40" s="25"/>
       <c r="B40" s="11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D40" s="13">
         <v>0.5</v>
@@ -2918,30 +2935,30 @@
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A41" s="20"/>
-      <c r="B41" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C41" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="D41" s="13">
+      <c r="A41" s="25"/>
+      <c r="B41" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="C41" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="D41" s="22">
         <v>0</v>
       </c>
-      <c r="E41" s="13">
+      <c r="E41" s="22">
         <v>0</v>
       </c>
-      <c r="F41" s="14">
+      <c r="F41" s="23">
         <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A42" s="20"/>
+      <c r="A42" s="25"/>
       <c r="B42" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D42" s="13">
         <v>2</v>
@@ -2954,48 +2971,48 @@
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43" s="20"/>
+      <c r="A43" s="25"/>
       <c r="B43" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C43" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D43" s="13">
+        <v>1</v>
+      </c>
+      <c r="E43" s="13">
+        <v>1</v>
+      </c>
+      <c r="F43" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" s="25"/>
+      <c r="B44" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C43" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="D43" s="13">
-        <v>1</v>
-      </c>
-      <c r="E43" s="13">
-        <v>1</v>
-      </c>
-      <c r="F43" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A44" s="20"/>
-      <c r="B44" s="11" t="s">
+      <c r="C44" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D44" s="13">
+        <v>1</v>
+      </c>
+      <c r="E44" s="13">
+        <v>1</v>
+      </c>
+      <c r="F44" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" s="25"/>
+      <c r="B45" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C44" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="D44" s="13">
-        <v>1</v>
-      </c>
-      <c r="E44" s="13">
-        <v>1</v>
-      </c>
-      <c r="F44" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A45" s="20"/>
-      <c r="B45" s="11" t="s">
-        <v>12</v>
-      </c>
       <c r="C45" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D45" s="13">
         <v>1</v>
@@ -3008,12 +3025,12 @@
       </c>
     </row>
     <row r="46" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="21"/>
+      <c r="A46" s="26"/>
       <c r="B46" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C46" s="16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D46" s="17">
         <v>0.7</v>
@@ -3040,8 +3057,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34DC9FCA-E070-744D-A42B-CA7E9735447B}">
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView topLeftCell="A4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3058,7 +3075,7 @@
         <v>4</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>1</v>
@@ -3071,158 +3088,158 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="19" t="s">
-        <v>17</v>
+      <c r="A2" s="24" t="s">
+        <v>16</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="20"/>
+      <c r="A3" s="25"/>
       <c r="B3" s="9" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="20"/>
+      <c r="A4" s="25"/>
       <c r="B4" s="11" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="25"/>
+      <c r="B5" s="11" t="s">
         <v>20</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="20"/>
-      <c r="B5" s="11" t="s">
-        <v>21</v>
       </c>
       <c r="C5" s="12">
         <v>8000</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="20"/>
+      <c r="A6" s="25"/>
       <c r="B6" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C6" s="12">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="20"/>
+      <c r="A7" s="25"/>
       <c r="B7" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C7" s="12">
         <v>8</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F7" s="14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="20"/>
+      <c r="A8" s="25"/>
       <c r="B8" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C8" s="12">
         <v>8</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="20"/>
+      <c r="A9" s="25"/>
       <c r="B9" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D9" s="13">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="E9" s="13">
-        <v>2</v>
-      </c>
-      <c r="F9" s="14">
-        <v>2</v>
+        <v>12</v>
+      </c>
+      <c r="F9" s="13">
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="20"/>
+      <c r="A10" s="25"/>
       <c r="B10" s="11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D10" s="13">
         <v>0.5</v>
@@ -3235,30 +3252,30 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="20"/>
-      <c r="B11" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="13">
+      <c r="A11" s="25"/>
+      <c r="B11" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="22">
         <v>0</v>
       </c>
-      <c r="E11" s="13">
+      <c r="E11" s="22">
         <v>0</v>
       </c>
-      <c r="F11" s="14">
+      <c r="F11" s="23">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="20"/>
+      <c r="A12" s="25"/>
       <c r="B12" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D12" s="13">
         <v>2</v>
@@ -3271,48 +3288,48 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="20"/>
+      <c r="A13" s="25"/>
       <c r="B13" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="13">
+        <v>1</v>
+      </c>
+      <c r="E13" s="13">
+        <v>1</v>
+      </c>
+      <c r="F13" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="25"/>
+      <c r="B14" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13" s="13">
-        <v>0</v>
-      </c>
-      <c r="E13" s="13">
-        <v>0</v>
-      </c>
-      <c r="F13" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="20"/>
-      <c r="B14" s="11" t="s">
+      <c r="C14" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="13">
+        <v>1</v>
+      </c>
+      <c r="E14" s="13">
+        <v>1</v>
+      </c>
+      <c r="F14" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="25"/>
+      <c r="B15" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="D14" s="13">
-        <v>1</v>
-      </c>
-      <c r="E14" s="13">
-        <v>1</v>
-      </c>
-      <c r="F14" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="20"/>
-      <c r="B15" s="11" t="s">
-        <v>12</v>
-      </c>
       <c r="C15" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D15" s="13">
         <v>1</v>
@@ -3325,12 +3342,12 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="21"/>
+      <c r="A16" s="26"/>
       <c r="B16" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D16" s="17">
         <v>0.7</v>
@@ -3343,158 +3360,158 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="19" t="s">
-        <v>18</v>
+      <c r="A17" s="24" t="s">
+        <v>17</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="20"/>
+      <c r="A18" s="25"/>
       <c r="B18" s="9" t="s">
         <v>5</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="20"/>
+      <c r="A19" s="25"/>
       <c r="B19" s="11" t="s">
         <v>6</v>
       </c>
       <c r="C19" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F19" s="14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="25"/>
+      <c r="B20" s="11" t="s">
         <v>20</v>
-      </c>
-      <c r="D19" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E19" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="F19" s="14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="20"/>
-      <c r="B20" s="11" t="s">
-        <v>21</v>
       </c>
       <c r="C20" s="12">
         <v>8000</v>
       </c>
       <c r="D20" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E20" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F20" s="14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="20"/>
+      <c r="A21" s="25"/>
       <c r="B21" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C21" s="12">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="D21" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E21" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F21" s="14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="20"/>
+      <c r="A22" s="25"/>
       <c r="B22" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C22" s="12">
         <v>8</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E22" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F22" s="14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="20"/>
+      <c r="A23" s="25"/>
       <c r="B23" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C23" s="12">
         <v>8</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E23" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F23" s="14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="20"/>
+      <c r="A24" s="25"/>
       <c r="B24" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D24" s="13">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="E24" s="13">
-        <v>2</v>
-      </c>
-      <c r="F24" s="14">
-        <v>2</v>
+        <v>12</v>
+      </c>
+      <c r="F24" s="13">
+        <v>12</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="20"/>
+      <c r="A25" s="25"/>
       <c r="B25" s="11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D25" s="13">
         <v>0.5</v>
@@ -3507,30 +3524,30 @@
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="20"/>
-      <c r="B26" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C26" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="D26" s="13">
+      <c r="A26" s="25"/>
+      <c r="B26" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="D26" s="22">
         <v>0</v>
       </c>
-      <c r="E26" s="13">
+      <c r="E26" s="22">
         <v>0</v>
       </c>
-      <c r="F26" s="14">
+      <c r="F26" s="23">
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="20"/>
+      <c r="A27" s="25"/>
       <c r="B27" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D27" s="13">
         <v>2</v>
@@ -3543,48 +3560,48 @@
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" s="20"/>
+      <c r="A28" s="25"/>
       <c r="B28" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D28" s="13">
+        <v>1</v>
+      </c>
+      <c r="E28" s="13">
+        <v>1</v>
+      </c>
+      <c r="F28" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" s="25"/>
+      <c r="B29" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C28" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="D28" s="13">
-        <v>0</v>
-      </c>
-      <c r="E28" s="13">
-        <v>0</v>
-      </c>
-      <c r="F28" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" s="20"/>
-      <c r="B29" s="11" t="s">
+      <c r="C29" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D29" s="13">
+        <v>1</v>
+      </c>
+      <c r="E29" s="13">
+        <v>1</v>
+      </c>
+      <c r="F29" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" s="25"/>
+      <c r="B30" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C29" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="D29" s="13">
-        <v>1</v>
-      </c>
-      <c r="E29" s="13">
-        <v>1</v>
-      </c>
-      <c r="F29" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30" s="20"/>
-      <c r="B30" s="11" t="s">
-        <v>12</v>
-      </c>
       <c r="C30" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D30" s="13">
         <v>1</v>
@@ -3597,12 +3614,12 @@
       </c>
     </row>
     <row r="31" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="21"/>
+      <c r="A31" s="26"/>
       <c r="B31" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C31" s="16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D31" s="17">
         <v>0.7</v>
@@ -3615,158 +3632,158 @@
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" s="19" t="s">
-        <v>19</v>
+      <c r="A32" s="24" t="s">
+        <v>18</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F32" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33" s="20"/>
+      <c r="A33" s="25"/>
       <c r="B33" s="9" t="s">
         <v>5</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F33" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34" s="20"/>
+      <c r="A34" s="25"/>
       <c r="B34" s="11" t="s">
         <v>6</v>
       </c>
       <c r="C34" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D34" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E34" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F34" s="14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" s="25"/>
+      <c r="B35" s="11" t="s">
         <v>20</v>
-      </c>
-      <c r="D34" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E34" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="F34" s="14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35" s="20"/>
-      <c r="B35" s="11" t="s">
-        <v>21</v>
       </c>
       <c r="C35" s="12">
         <v>8000</v>
       </c>
       <c r="D35" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E35" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F35" s="14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36" s="20"/>
+      <c r="A36" s="25"/>
       <c r="B36" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C36" s="12">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="D36" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E36" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F36" s="14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37" s="20"/>
+      <c r="A37" s="25"/>
       <c r="B37" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C37" s="12">
         <v>8</v>
       </c>
       <c r="D37" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E37" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F37" s="14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38" s="20"/>
+      <c r="A38" s="25"/>
       <c r="B38" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C38" s="12">
         <v>8</v>
       </c>
       <c r="D38" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E38" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F38" s="14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A39" s="20"/>
+      <c r="A39" s="25"/>
       <c r="B39" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D39" s="13">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="E39" s="13">
-        <v>2</v>
-      </c>
-      <c r="F39" s="14">
-        <v>2</v>
+        <v>12</v>
+      </c>
+      <c r="F39" s="13">
+        <v>12</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A40" s="20"/>
+      <c r="A40" s="25"/>
       <c r="B40" s="11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D40" s="13">
         <v>0.5</v>
@@ -3779,30 +3796,31 @@
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A41" s="20"/>
-      <c r="B41" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C41" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="D41" s="13">
+      <c r="A41" s="25"/>
+      <c r="B41" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="C41" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="D41" s="22">
         <v>0</v>
       </c>
-      <c r="E41" s="13">
+      <c r="E41" s="22">
         <v>0</v>
       </c>
-      <c r="F41" s="14">
+      <c r="F41" s="23">
+        <f>-F110</f>
         <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A42" s="20"/>
+      <c r="A42" s="25"/>
       <c r="B42" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D42" s="13">
         <v>2</v>
@@ -3815,48 +3833,48 @@
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43" s="20"/>
+      <c r="A43" s="25"/>
       <c r="B43" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C43" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D43" s="13">
+        <v>1</v>
+      </c>
+      <c r="E43" s="13">
+        <v>1</v>
+      </c>
+      <c r="F43" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" s="25"/>
+      <c r="B44" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C43" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="D43" s="13">
-        <v>0</v>
-      </c>
-      <c r="E43" s="13">
-        <v>0</v>
-      </c>
-      <c r="F43" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A44" s="20"/>
-      <c r="B44" s="11" t="s">
+      <c r="C44" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D44" s="13">
+        <v>1</v>
+      </c>
+      <c r="E44" s="13">
+        <v>1</v>
+      </c>
+      <c r="F44" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" s="25"/>
+      <c r="B45" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C44" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="D44" s="13">
-        <v>1</v>
-      </c>
-      <c r="E44" s="13">
-        <v>1</v>
-      </c>
-      <c r="F44" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A45" s="20"/>
-      <c r="B45" s="11" t="s">
-        <v>12</v>
-      </c>
       <c r="C45" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D45" s="13">
         <v>1</v>
@@ -3869,12 +3887,12 @@
       </c>
     </row>
     <row r="46" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="21"/>
+      <c r="A46" s="26"/>
       <c r="B46" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C46" s="16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D46" s="17">
         <v>0.7</v>

</xml_diff>